<commit_message>
UI-821: Correct steps' references
</commit_message>
<xml_diff>
--- a/design/Test Plan/TestPlan.xlsx
+++ b/design/Test Plan/TestPlan.xlsx
@@ -829,9 +829,6 @@
     <t>A dialog window will open and a section containing a dropwdown will appear in the dialog</t>
   </si>
   <si>
-    <t>To upload a new file follow steps from 14B to 14C</t>
-  </si>
-  <si>
     <t>The new file will appear in the dropdown</t>
   </si>
   <si>
@@ -901,9 +898,6 @@
     <t>Click on the "Advanced" button, select the "Video" option and drag and drop items from one table to the other</t>
   </si>
   <si>
-    <t>Same expectation as step 21E</t>
-  </si>
-  <si>
     <t>Click on the "Advanced" button, and select the "Restrictions" option</t>
   </si>
   <si>
@@ -952,9 +946,6 @@
     <t>A dialog window will open containing a list of device's brand</t>
   </si>
   <si>
-    <t>Click on the "The brand o f my device is not listed here"</t>
-  </si>
-  <si>
     <t>Come back to the brand listing dialog window and choose one by clicking on it</t>
   </si>
   <si>
@@ -964,9 +955,6 @@
     <t>Click on the "My device is not listed here"</t>
   </si>
   <si>
-    <t>Follow steps from 21C until the end of the test</t>
-  </si>
-  <si>
     <t>Come back to the device listing dialog window and choose one by clicking on it</t>
   </si>
   <si>
@@ -1415,6 +1403,18 @@
   </si>
   <si>
     <t>The "Incoming Call Handling" section will close and a notification will inform you that the strategy was successfully updated</t>
+  </si>
+  <si>
+    <t>Click on the "The brand of my device is not listed here"</t>
+  </si>
+  <si>
+    <t>Same expectation as step 29E</t>
+  </si>
+  <si>
+    <t>Follow steps from 29C until the end of the test</t>
+  </si>
+  <si>
+    <t>To upload a new file follow steps from 21B to 21C</t>
   </si>
 </sst>
 </file>
@@ -1873,15 +1873,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1914,6 +1905,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2227,8 +2227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L392"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D102" sqref="D102"/>
+    <sheetView tabSelected="1" topLeftCell="A309" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D317" sqref="D317"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2249,51 +2249,51 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="26.45" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="75"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="72"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="79"/>
+      <c r="C3" s="76"/>
       <c r="D3" s="11" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="80" t="s">
+      <c r="B4" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="81"/>
+      <c r="C4" s="78"/>
       <c r="D4" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="82" t="s">
+      <c r="B5" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="83"/>
+      <c r="C5" s="80"/>
       <c r="D5" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="76" t="s">
+      <c r="B6" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="77"/>
+      <c r="C6" s="74"/>
       <c r="D6" s="19"/>
     </row>
     <row r="7" spans="2:12" s="3" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="76" t="s">
+      <c r="B7" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="77"/>
+      <c r="C7" s="74"/>
       <c r="D7" s="23" t="s">
         <v>24</v>
       </c>
@@ -2301,17 +2301,17 @@
       <c r="L7" s="2"/>
     </row>
     <row r="8" spans="2:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="76" t="s">
+      <c r="B8" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="77"/>
+      <c r="C8" s="74"/>
       <c r="D8" s="13"/>
     </row>
     <row r="10" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="56"/>
       <c r="D10" s="56"/>
       <c r="E10" s="59" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="F10" s="56"/>
       <c r="G10" s="56"/>
@@ -2338,7 +2338,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="43" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="E13" s="44"/>
       <c r="F13" s="44"/>
@@ -2390,10 +2390,10 @@
         <v>10</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="F16" s="16"/>
       <c r="G16" s="18" t="s">
@@ -2412,10 +2412,10 @@
         <v>11</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="E17" s="27" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="F17" s="28"/>
       <c r="G17" s="29" t="s">
@@ -2434,10 +2434,10 @@
         <v>12</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="21" t="s">
@@ -2456,10 +2456,10 @@
         <v>22</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="E19" s="27" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="F19" s="28"/>
       <c r="G19" s="29" t="s">
@@ -2478,10 +2478,10 @@
         <v>27</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="F20" s="16"/>
       <c r="G20" s="18" t="s">
@@ -2500,10 +2500,10 @@
         <v>28</v>
       </c>
       <c r="D21" s="33" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="E21" s="27" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F21" s="28"/>
       <c r="G21" s="29" t="s">
@@ -2536,7 +2536,7 @@
         <v>2</v>
       </c>
       <c r="D24" s="43" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E24" s="44"/>
       <c r="F24" s="44"/>
@@ -2588,10 +2588,10 @@
         <v>10</v>
       </c>
       <c r="D27" s="32" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="F27" s="16"/>
       <c r="G27" s="18" t="s">
@@ -2610,10 +2610,10 @@
         <v>11</v>
       </c>
       <c r="D28" s="33" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="E28" s="27" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="F28" s="28"/>
       <c r="G28" s="29" t="s">
@@ -2665,12 +2665,12 @@
       <c r="E32" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="F32" s="70" t="s">
+      <c r="F32" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="G32" s="71"/>
-      <c r="H32" s="71"/>
-      <c r="I32" s="72"/>
+      <c r="G32" s="82"/>
+      <c r="H32" s="82"/>
+      <c r="I32" s="83"/>
       <c r="J32" s="68" t="s">
         <v>8</v>
       </c>
@@ -2698,10 +2698,10 @@
         <v>10</v>
       </c>
       <c r="D34" s="32" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="F34" s="16"/>
       <c r="G34" s="18" t="s">
@@ -2720,10 +2720,10 @@
         <v>11</v>
       </c>
       <c r="D35" s="33" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="E35" s="27" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="F35" s="28"/>
       <c r="G35" s="29" t="s">
@@ -2742,7 +2742,7 @@
         <v>12</v>
       </c>
       <c r="D36" s="34" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>206</v>
@@ -2764,10 +2764,10 @@
         <v>22</v>
       </c>
       <c r="D37" s="33" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="E37" s="27" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="F37" s="28"/>
       <c r="G37" s="29" t="s">
@@ -2785,7 +2785,7 @@
       <c r="C39" s="56"/>
       <c r="D39" s="56"/>
       <c r="E39" s="59" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="F39" s="56"/>
       <c r="G39" s="56"/>
@@ -2812,7 +2812,7 @@
         <v>4</v>
       </c>
       <c r="D42" s="43" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="E42" s="44"/>
       <c r="F42" s="44"/>
@@ -2864,10 +2864,10 @@
         <v>10</v>
       </c>
       <c r="D45" s="32" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="F45" s="16"/>
       <c r="G45" s="18" t="s">
@@ -2886,10 +2886,10 @@
         <v>11</v>
       </c>
       <c r="D46" s="33" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="E46" s="27" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F46" s="28"/>
       <c r="G46" s="29" t="s">
@@ -2908,10 +2908,10 @@
         <v>12</v>
       </c>
       <c r="D47" s="34" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="F47" s="17"/>
       <c r="G47" s="21" t="s">
@@ -2930,10 +2930,10 @@
         <v>22</v>
       </c>
       <c r="D48" s="33" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="E48" s="27" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="F48" s="28"/>
       <c r="G48" s="29" t="s">
@@ -2952,10 +2952,10 @@
         <v>27</v>
       </c>
       <c r="D49" s="32" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="F49" s="16"/>
       <c r="G49" s="18" t="s">
@@ -2977,7 +2977,7 @@
         <v>121</v>
       </c>
       <c r="E50" s="27" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="F50" s="28"/>
       <c r="G50" s="29" t="s">
@@ -2996,10 +2996,10 @@
         <v>29</v>
       </c>
       <c r="D51" s="35" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="E51" s="36" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="F51" s="25"/>
       <c r="G51" s="26" t="s">
@@ -3032,7 +3032,7 @@
         <v>5</v>
       </c>
       <c r="D54" s="43" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="E54" s="44"/>
       <c r="F54" s="44"/>
@@ -3084,10 +3084,10 @@
         <v>10</v>
       </c>
       <c r="D57" s="32" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="F57" s="16"/>
       <c r="G57" s="18" t="s">
@@ -3106,10 +3106,10 @@
         <v>11</v>
       </c>
       <c r="D58" s="33" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="E58" s="27" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="F58" s="28"/>
       <c r="G58" s="29" t="s">
@@ -3128,10 +3128,10 @@
         <v>12</v>
       </c>
       <c r="D59" s="34" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="F59" s="17"/>
       <c r="G59" s="21" t="s">
@@ -3150,10 +3150,10 @@
         <v>22</v>
       </c>
       <c r="D60" s="33" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="E60" s="27" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="F60" s="28"/>
       <c r="G60" s="29" t="s">
@@ -3172,10 +3172,10 @@
         <v>27</v>
       </c>
       <c r="D61" s="32" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="F61" s="16"/>
       <c r="G61" s="18" t="s">
@@ -3197,7 +3197,7 @@
         <v>134</v>
       </c>
       <c r="E62" s="27" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="F62" s="28"/>
       <c r="G62" s="29" t="s">
@@ -3230,7 +3230,7 @@
         <v>6</v>
       </c>
       <c r="D65" s="43" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="E65" s="44"/>
       <c r="F65" s="44"/>
@@ -3282,10 +3282,10 @@
         <v>10</v>
       </c>
       <c r="D68" s="32" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="F68" s="16"/>
       <c r="G68" s="18" t="s">
@@ -3304,10 +3304,10 @@
         <v>11</v>
       </c>
       <c r="D69" s="33" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="E69" s="27" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="F69" s="28"/>
       <c r="G69" s="29" t="s">
@@ -3326,10 +3326,10 @@
         <v>12</v>
       </c>
       <c r="D70" s="34" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F70" s="17"/>
       <c r="G70" s="21" t="s">
@@ -3348,10 +3348,10 @@
         <v>22</v>
       </c>
       <c r="D71" s="33" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="E71" s="27" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="F71" s="28"/>
       <c r="G71" s="29" t="s">
@@ -3370,10 +3370,10 @@
         <v>27</v>
       </c>
       <c r="D72" s="32" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="F72" s="16"/>
       <c r="G72" s="18" t="s">
@@ -3392,10 +3392,10 @@
         <v>28</v>
       </c>
       <c r="D73" s="33" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="E73" s="27" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="F73" s="28"/>
       <c r="G73" s="29" t="s">
@@ -3414,10 +3414,10 @@
         <v>29</v>
       </c>
       <c r="D74" s="32" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="F74" s="16"/>
       <c r="G74" s="18" t="s">
@@ -3436,10 +3436,10 @@
         <v>30</v>
       </c>
       <c r="D75" s="33" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="E75" s="27" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="F75" s="28"/>
       <c r="G75" s="29" t="s">
@@ -3458,10 +3458,10 @@
         <v>31</v>
       </c>
       <c r="D76" s="32" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="F76" s="16"/>
       <c r="G76" s="18" t="s">
@@ -3480,10 +3480,10 @@
         <v>32</v>
       </c>
       <c r="D77" s="33" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="E77" s="27" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="F77" s="28"/>
       <c r="G77" s="29" t="s">
@@ -3505,7 +3505,7 @@
         <v>134</v>
       </c>
       <c r="E78" s="7" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F78" s="17"/>
       <c r="G78" s="21" t="s">
@@ -3538,7 +3538,7 @@
         <v>7</v>
       </c>
       <c r="D81" s="43" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="E81" s="44"/>
       <c r="F81" s="44"/>
@@ -3590,10 +3590,10 @@
         <v>10</v>
       </c>
       <c r="D84" s="32" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="F84" s="16"/>
       <c r="G84" s="18" t="s">
@@ -3612,10 +3612,10 @@
         <v>11</v>
       </c>
       <c r="D85" s="33" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="E85" s="27" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="F85" s="28"/>
       <c r="G85" s="29" t="s">
@@ -3634,10 +3634,10 @@
         <v>12</v>
       </c>
       <c r="D86" s="35" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="E86" s="7" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="F86" s="17"/>
       <c r="G86" s="21" t="s">
@@ -3656,10 +3656,10 @@
         <v>22</v>
       </c>
       <c r="D87" s="33" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="E87" s="27" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="F87" s="28"/>
       <c r="G87" s="29" t="s">
@@ -3678,10 +3678,10 @@
         <v>27</v>
       </c>
       <c r="D88" s="32" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="F88" s="16"/>
       <c r="G88" s="18" t="s">
@@ -3700,10 +3700,10 @@
         <v>28</v>
       </c>
       <c r="D89" s="33" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="E89" s="27" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="F89" s="28"/>
       <c r="G89" s="29" t="s">
@@ -3722,10 +3722,10 @@
         <v>29</v>
       </c>
       <c r="D90" s="32" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="F90" s="16"/>
       <c r="G90" s="18" t="s">
@@ -3744,10 +3744,10 @@
         <v>30</v>
       </c>
       <c r="D91" s="33" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="E91" s="27" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="F91" s="28"/>
       <c r="G91" s="29" t="s">
@@ -3766,10 +3766,10 @@
         <v>31</v>
       </c>
       <c r="D92" s="32" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="E92" s="9" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="F92" s="16"/>
       <c r="G92" s="18" t="s">
@@ -3788,10 +3788,10 @@
         <v>32</v>
       </c>
       <c r="D93" s="33" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="E93" s="27" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="F93" s="28"/>
       <c r="G93" s="29" t="s">
@@ -3810,10 +3810,10 @@
         <v>33</v>
       </c>
       <c r="D94" s="34" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="F94" s="17"/>
       <c r="G94" s="21" t="s">
@@ -3835,7 +3835,7 @@
         <v>134</v>
       </c>
       <c r="E95" s="27" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="F95" s="28"/>
       <c r="G95" s="29" t="s">
@@ -3868,7 +3868,7 @@
         <v>8</v>
       </c>
       <c r="D98" s="43" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="E98" s="44"/>
       <c r="F98" s="44"/>
@@ -3920,10 +3920,10 @@
         <v>10</v>
       </c>
       <c r="D101" s="32" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="E101" s="9" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="F101" s="16"/>
       <c r="G101" s="18" t="s">
@@ -3942,10 +3942,10 @@
         <v>11</v>
       </c>
       <c r="D102" s="33" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="E102" s="27" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="F102" s="28"/>
       <c r="G102" s="29" t="s">
@@ -3964,10 +3964,10 @@
         <v>12</v>
       </c>
       <c r="D103" s="34" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="F103" s="17"/>
       <c r="G103" s="21" t="s">
@@ -3986,10 +3986,10 @@
         <v>22</v>
       </c>
       <c r="D104" s="33" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="E104" s="27" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="F104" s="28"/>
       <c r="G104" s="29" t="s">
@@ -4007,7 +4007,7 @@
       <c r="C106" s="56"/>
       <c r="D106" s="56"/>
       <c r="E106" s="59" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="F106" s="56"/>
       <c r="G106" s="56"/>
@@ -6901,7 +6901,7 @@
       <c r="C269" s="56"/>
       <c r="D269" s="56"/>
       <c r="E269" s="59" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="F269" s="56"/>
       <c r="G269" s="56"/>
@@ -7486,10 +7486,10 @@
         <v>39</v>
       </c>
       <c r="D300" s="35" t="s">
+        <v>280</v>
+      </c>
+      <c r="E300" s="36" t="s">
         <v>281</v>
-      </c>
-      <c r="E300" s="36" t="s">
-        <v>282</v>
       </c>
       <c r="F300" s="25"/>
       <c r="G300" s="26" t="s">
@@ -7665,7 +7665,7 @@
         <v>267</v>
       </c>
       <c r="E310" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F310" s="17"/>
       <c r="G310" s="21" t="s">
@@ -7772,10 +7772,10 @@
         <v>11</v>
       </c>
       <c r="D317" s="33" t="s">
+        <v>466</v>
+      </c>
+      <c r="E317" s="27" t="s">
         <v>271</v>
-      </c>
-      <c r="E317" s="27" t="s">
-        <v>272</v>
       </c>
       <c r="F317" s="28"/>
       <c r="G317" s="29" t="s">
@@ -7794,7 +7794,7 @@
         <v>12</v>
       </c>
       <c r="D318" s="34" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E318" s="7" t="s">
         <v>265</v>
@@ -7816,10 +7816,10 @@
         <v>22</v>
       </c>
       <c r="D319" s="33" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E319" s="27" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F319" s="28"/>
       <c r="G319" s="29" t="s">
@@ -7852,7 +7852,7 @@
         <v>28</v>
       </c>
       <c r="D322" s="43" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E322" s="44"/>
       <c r="F322" s="44"/>
@@ -7904,10 +7904,10 @@
         <v>10</v>
       </c>
       <c r="D325" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="E325" s="9" t="s">
         <v>277</v>
-      </c>
-      <c r="E325" s="9" t="s">
-        <v>278</v>
       </c>
       <c r="F325" s="16"/>
       <c r="G325" s="18" t="s">
@@ -7948,10 +7948,10 @@
         <v>12</v>
       </c>
       <c r="D327" s="34" t="s">
+        <v>278</v>
+      </c>
+      <c r="E327" s="7" t="s">
         <v>279</v>
-      </c>
-      <c r="E327" s="7" t="s">
-        <v>280</v>
       </c>
       <c r="F327" s="17"/>
       <c r="G327" s="21" t="s">
@@ -7969,7 +7969,7 @@
       <c r="C329" s="56"/>
       <c r="D329" s="56"/>
       <c r="E329" s="59" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F329" s="56"/>
       <c r="G329" s="56"/>
@@ -7996,7 +7996,7 @@
         <v>29</v>
       </c>
       <c r="D332" s="43" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E332" s="44"/>
       <c r="F332" s="44"/>
@@ -8048,10 +8048,10 @@
         <v>10</v>
       </c>
       <c r="D335" s="32" t="s">
+        <v>282</v>
+      </c>
+      <c r="E335" s="9" t="s">
         <v>283</v>
-      </c>
-      <c r="E335" s="9" t="s">
-        <v>284</v>
       </c>
       <c r="F335" s="16"/>
       <c r="G335" s="18" t="s">
@@ -8070,10 +8070,10 @@
         <v>11</v>
       </c>
       <c r="D336" s="33" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E336" s="27" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F336" s="28"/>
       <c r="G336" s="29" t="s">
@@ -8092,10 +8092,10 @@
         <v>12</v>
       </c>
       <c r="D337" s="34" t="s">
+        <v>287</v>
+      </c>
+      <c r="E337" s="7" t="s">
         <v>288</v>
-      </c>
-      <c r="E337" s="7" t="s">
-        <v>289</v>
       </c>
       <c r="F337" s="17"/>
       <c r="G337" s="21" t="s">
@@ -8114,10 +8114,10 @@
         <v>22</v>
       </c>
       <c r="D338" s="33" t="s">
+        <v>289</v>
+      </c>
+      <c r="E338" s="27" t="s">
         <v>290</v>
-      </c>
-      <c r="E338" s="27" t="s">
-        <v>291</v>
       </c>
       <c r="F338" s="28"/>
       <c r="G338" s="29" t="s">
@@ -8136,10 +8136,10 @@
         <v>27</v>
       </c>
       <c r="D339" s="32" t="s">
+        <v>291</v>
+      </c>
+      <c r="E339" s="9" t="s">
         <v>292</v>
-      </c>
-      <c r="E339" s="9" t="s">
-        <v>293</v>
       </c>
       <c r="F339" s="16"/>
       <c r="G339" s="18" t="s">
@@ -8158,10 +8158,10 @@
         <v>28</v>
       </c>
       <c r="D340" s="33" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E340" s="27" t="s">
-        <v>295</v>
+        <v>464</v>
       </c>
       <c r="F340" s="28"/>
       <c r="G340" s="29" t="s">
@@ -8180,10 +8180,10 @@
         <v>29</v>
       </c>
       <c r="D341" s="32" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E341" s="9" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F341" s="16"/>
       <c r="G341" s="18" t="s">
@@ -8202,10 +8202,10 @@
         <v>30</v>
       </c>
       <c r="D342" s="33" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E342" s="27" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F342" s="28"/>
       <c r="G342" s="29" t="s">
@@ -8224,10 +8224,10 @@
         <v>31</v>
       </c>
       <c r="D343" s="32" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E343" s="9" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F343" s="16"/>
       <c r="G343" s="18" t="s">
@@ -8246,10 +8246,10 @@
         <v>32</v>
       </c>
       <c r="D344" s="33" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E344" s="27" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F344" s="28"/>
       <c r="G344" s="29" t="s">
@@ -8268,10 +8268,10 @@
         <v>33</v>
       </c>
       <c r="D345" s="34" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E345" s="7" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F345" s="17"/>
       <c r="G345" s="21" t="s">
@@ -8290,10 +8290,10 @@
         <v>34</v>
       </c>
       <c r="D346" s="33" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E346" s="27" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F346" s="28"/>
       <c r="G346" s="29" t="s">
@@ -8312,10 +8312,10 @@
         <v>35</v>
       </c>
       <c r="D347" s="35" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E347" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F347" s="25"/>
       <c r="G347" s="26" t="s">
@@ -8348,7 +8348,7 @@
         <v>30</v>
       </c>
       <c r="D350" s="43" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E350" s="44"/>
       <c r="F350" s="44"/>
@@ -8400,10 +8400,10 @@
         <v>10</v>
       </c>
       <c r="D353" s="32" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E353" s="9" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F353" s="16"/>
       <c r="G353" s="18" t="s">
@@ -8422,10 +8422,10 @@
         <v>11</v>
       </c>
       <c r="D354" s="33" t="s">
-        <v>312</v>
+        <v>463</v>
       </c>
       <c r="E354" s="27" t="s">
-        <v>316</v>
+        <v>465</v>
       </c>
       <c r="F354" s="28"/>
       <c r="G354" s="29" t="s">
@@ -8444,10 +8444,10 @@
         <v>12</v>
       </c>
       <c r="D355" s="34" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="E355" s="7" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="F355" s="17"/>
       <c r="G355" s="21" t="s">
@@ -8466,10 +8466,10 @@
         <v>22</v>
       </c>
       <c r="D356" s="33" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="E356" s="27" t="s">
-        <v>316</v>
+        <v>465</v>
       </c>
       <c r="F356" s="28"/>
       <c r="G356" s="29" t="s">
@@ -8488,10 +8488,10 @@
         <v>27</v>
       </c>
       <c r="D357" s="32" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="E357" s="9" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="F357" s="16"/>
       <c r="G357" s="18" t="s">
@@ -8510,10 +8510,10 @@
         <v>28</v>
       </c>
       <c r="D358" s="33" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="E358" s="27" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F358" s="28"/>
       <c r="G358" s="29" t="s">
@@ -8546,7 +8546,7 @@
         <v>31</v>
       </c>
       <c r="D361" s="43" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="E361" s="44"/>
       <c r="F361" s="44"/>
@@ -8598,10 +8598,10 @@
         <v>10</v>
       </c>
       <c r="D364" s="32" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="E364" s="9" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="F364" s="16"/>
       <c r="G364" s="18" t="s">
@@ -8620,10 +8620,10 @@
         <v>11</v>
       </c>
       <c r="D365" s="33" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="E365" s="27" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="F365" s="28"/>
       <c r="G365" s="29" t="s">
@@ -8645,7 +8645,7 @@
         <v>134</v>
       </c>
       <c r="E366" s="7" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="F366" s="17"/>
       <c r="G366" s="21" t="s">
@@ -8664,10 +8664,10 @@
         <v>22</v>
       </c>
       <c r="D367" s="33" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="E367" s="27" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="F367" s="28"/>
       <c r="G367" s="29" t="s">
@@ -8686,10 +8686,10 @@
         <v>27</v>
       </c>
       <c r="D368" s="32" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E368" s="9" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="F368" s="16"/>
       <c r="G368" s="18" t="s">
@@ -8708,10 +8708,10 @@
         <v>28</v>
       </c>
       <c r="D369" s="33" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="E369" s="27" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="F369" s="28"/>
       <c r="G369" s="29" t="s">
@@ -8733,7 +8733,7 @@
         <v>70</v>
       </c>
       <c r="E370" s="36" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="F370" s="25"/>
       <c r="G370" s="26" t="s">
@@ -8751,7 +8751,7 @@
       <c r="C372" s="56"/>
       <c r="D372" s="56"/>
       <c r="E372" s="59" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="F372" s="56"/>
       <c r="G372" s="56"/>
@@ -8778,7 +8778,7 @@
         <v>32</v>
       </c>
       <c r="D375" s="43" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="E375" s="44"/>
       <c r="F375" s="44"/>
@@ -8830,10 +8830,10 @@
         <v>10</v>
       </c>
       <c r="D378" s="32" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E378" s="9" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F378" s="16"/>
       <c r="G378" s="18" t="s">
@@ -8852,10 +8852,10 @@
         <v>11</v>
       </c>
       <c r="D379" s="33" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="E379" s="27" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="F379" s="28"/>
       <c r="G379" s="29" t="s">
@@ -8874,10 +8874,10 @@
         <v>12</v>
       </c>
       <c r="D380" s="34" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="E380" s="7" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="F380" s="17"/>
       <c r="G380" s="21" t="s">
@@ -8896,10 +8896,10 @@
         <v>22</v>
       </c>
       <c r="D381" s="33" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="E381" s="27" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="F381" s="28"/>
       <c r="G381" s="29" t="s">
@@ -8918,10 +8918,10 @@
         <v>27</v>
       </c>
       <c r="D382" s="32" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E382" s="9" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="F382" s="16"/>
       <c r="G382" s="18" t="s">
@@ -8940,10 +8940,10 @@
         <v>28</v>
       </c>
       <c r="D383" s="33" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="E383" s="27" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="F383" s="28"/>
       <c r="G383" s="29" t="s">
@@ -8962,10 +8962,10 @@
         <v>29</v>
       </c>
       <c r="D384" s="35" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="E384" s="36" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="F384" s="25"/>
       <c r="G384" s="26" t="s">
@@ -8998,7 +8998,7 @@
         <v>33</v>
       </c>
       <c r="D387" s="43" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="E387" s="44"/>
       <c r="F387" s="44"/>
@@ -9050,10 +9050,10 @@
         <v>10</v>
       </c>
       <c r="D390" s="32" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="E390" s="9" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="F390" s="16"/>
       <c r="G390" s="18" t="s">
@@ -9072,10 +9072,10 @@
         <v>11</v>
       </c>
       <c r="D391" s="33" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="E391" s="27" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F391" s="28"/>
       <c r="G391" s="29" t="s">
@@ -9094,10 +9094,10 @@
         <v>12</v>
       </c>
       <c r="D392" s="34" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="E392" s="7" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="F392" s="17"/>
       <c r="G392" s="21" t="s">
@@ -9113,71 +9113,89 @@
     </row>
   </sheetData>
   <mergeCells count="172">
-    <mergeCell ref="C282:C283"/>
-    <mergeCell ref="D282:D283"/>
-    <mergeCell ref="E282:E283"/>
-    <mergeCell ref="F282:I282"/>
-    <mergeCell ref="J282:J283"/>
-    <mergeCell ref="C263:C264"/>
-    <mergeCell ref="D263:D264"/>
-    <mergeCell ref="E263:E264"/>
-    <mergeCell ref="F263:I263"/>
-    <mergeCell ref="J263:J264"/>
-    <mergeCell ref="C273:C274"/>
-    <mergeCell ref="D273:D274"/>
-    <mergeCell ref="E273:E274"/>
-    <mergeCell ref="F273:I273"/>
-    <mergeCell ref="J273:J274"/>
-    <mergeCell ref="C240:C241"/>
-    <mergeCell ref="D240:D241"/>
-    <mergeCell ref="E240:E241"/>
-    <mergeCell ref="F240:I240"/>
-    <mergeCell ref="J240:J241"/>
-    <mergeCell ref="C253:C254"/>
-    <mergeCell ref="D253:D254"/>
-    <mergeCell ref="E253:E254"/>
-    <mergeCell ref="F253:I253"/>
-    <mergeCell ref="J253:J254"/>
-    <mergeCell ref="C223:C224"/>
-    <mergeCell ref="D223:D224"/>
-    <mergeCell ref="E223:E224"/>
-    <mergeCell ref="F223:I223"/>
-    <mergeCell ref="J223:J224"/>
-    <mergeCell ref="C232:C233"/>
-    <mergeCell ref="D232:D233"/>
-    <mergeCell ref="E232:E233"/>
-    <mergeCell ref="F232:I232"/>
-    <mergeCell ref="J232:J233"/>
-    <mergeCell ref="C206:C207"/>
-    <mergeCell ref="D206:D207"/>
-    <mergeCell ref="E206:E207"/>
-    <mergeCell ref="F206:I206"/>
-    <mergeCell ref="J206:J207"/>
-    <mergeCell ref="C215:C216"/>
-    <mergeCell ref="D215:D216"/>
-    <mergeCell ref="E215:E216"/>
-    <mergeCell ref="F215:I215"/>
-    <mergeCell ref="J215:J216"/>
-    <mergeCell ref="C186:C187"/>
-    <mergeCell ref="D186:D187"/>
-    <mergeCell ref="E186:E187"/>
-    <mergeCell ref="F186:I186"/>
-    <mergeCell ref="J186:J187"/>
-    <mergeCell ref="C196:C197"/>
-    <mergeCell ref="D196:D197"/>
-    <mergeCell ref="E196:E197"/>
-    <mergeCell ref="F196:I196"/>
-    <mergeCell ref="J196:J197"/>
-    <mergeCell ref="C149:C150"/>
-    <mergeCell ref="D149:D150"/>
-    <mergeCell ref="E149:E150"/>
-    <mergeCell ref="F149:I149"/>
-    <mergeCell ref="J149:J150"/>
-    <mergeCell ref="C175:C176"/>
-    <mergeCell ref="D175:D176"/>
-    <mergeCell ref="E175:E176"/>
-    <mergeCell ref="F175:I175"/>
-    <mergeCell ref="J175:J176"/>
+    <mergeCell ref="C99:C100"/>
+    <mergeCell ref="D99:D100"/>
+    <mergeCell ref="E99:E100"/>
+    <mergeCell ref="F99:I99"/>
+    <mergeCell ref="J99:J100"/>
+    <mergeCell ref="D82:D83"/>
+    <mergeCell ref="E82:E83"/>
+    <mergeCell ref="F82:I82"/>
+    <mergeCell ref="J82:J83"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="F55:I55"/>
+    <mergeCell ref="J55:J56"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="E66:E67"/>
+    <mergeCell ref="F66:I66"/>
+    <mergeCell ref="J66:J67"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="J43:J44"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="J32:J33"/>
+    <mergeCell ref="C388:C389"/>
+    <mergeCell ref="D388:D389"/>
+    <mergeCell ref="E388:E389"/>
+    <mergeCell ref="F388:I388"/>
+    <mergeCell ref="J388:J389"/>
+    <mergeCell ref="C376:C377"/>
+    <mergeCell ref="D376:D377"/>
+    <mergeCell ref="E376:E377"/>
+    <mergeCell ref="F376:I376"/>
+    <mergeCell ref="J376:J377"/>
+    <mergeCell ref="C362:C363"/>
+    <mergeCell ref="D362:D363"/>
+    <mergeCell ref="E362:E363"/>
+    <mergeCell ref="F362:I362"/>
+    <mergeCell ref="J362:J363"/>
+    <mergeCell ref="C351:C352"/>
+    <mergeCell ref="D351:D352"/>
+    <mergeCell ref="E351:E352"/>
+    <mergeCell ref="F351:I351"/>
+    <mergeCell ref="J351:J352"/>
+    <mergeCell ref="C333:C334"/>
+    <mergeCell ref="D333:D334"/>
+    <mergeCell ref="E333:E334"/>
+    <mergeCell ref="F333:I333"/>
+    <mergeCell ref="J333:J334"/>
+    <mergeCell ref="C323:C324"/>
+    <mergeCell ref="D323:D324"/>
+    <mergeCell ref="E323:E324"/>
+    <mergeCell ref="F323:I323"/>
+    <mergeCell ref="J323:J324"/>
+    <mergeCell ref="C314:C315"/>
+    <mergeCell ref="D314:D315"/>
+    <mergeCell ref="E314:E315"/>
+    <mergeCell ref="F314:I314"/>
+    <mergeCell ref="J314:J315"/>
+    <mergeCell ref="C306:C307"/>
+    <mergeCell ref="D306:D307"/>
+    <mergeCell ref="E306:E307"/>
+    <mergeCell ref="F306:I306"/>
+    <mergeCell ref="J306:J307"/>
+    <mergeCell ref="C139:C140"/>
+    <mergeCell ref="D139:D140"/>
+    <mergeCell ref="E139:E140"/>
+    <mergeCell ref="F139:I139"/>
+    <mergeCell ref="J139:J140"/>
+    <mergeCell ref="C131:C132"/>
+    <mergeCell ref="D131:D132"/>
+    <mergeCell ref="E131:E132"/>
+    <mergeCell ref="F131:I131"/>
+    <mergeCell ref="J131:J132"/>
     <mergeCell ref="C120:C121"/>
     <mergeCell ref="D120:D121"/>
     <mergeCell ref="E120:E121"/>
@@ -9195,56 +9213,6 @@
     <mergeCell ref="E110:E111"/>
     <mergeCell ref="F110:I110"/>
     <mergeCell ref="J110:J111"/>
-    <mergeCell ref="C139:C140"/>
-    <mergeCell ref="D139:D140"/>
-    <mergeCell ref="E139:E140"/>
-    <mergeCell ref="F139:I139"/>
-    <mergeCell ref="J139:J140"/>
-    <mergeCell ref="C131:C132"/>
-    <mergeCell ref="D131:D132"/>
-    <mergeCell ref="E131:E132"/>
-    <mergeCell ref="F131:I131"/>
-    <mergeCell ref="J131:J132"/>
-    <mergeCell ref="C314:C315"/>
-    <mergeCell ref="D314:D315"/>
-    <mergeCell ref="E314:E315"/>
-    <mergeCell ref="F314:I314"/>
-    <mergeCell ref="J314:J315"/>
-    <mergeCell ref="C306:C307"/>
-    <mergeCell ref="D306:D307"/>
-    <mergeCell ref="E306:E307"/>
-    <mergeCell ref="F306:I306"/>
-    <mergeCell ref="J306:J307"/>
-    <mergeCell ref="C333:C334"/>
-    <mergeCell ref="D333:D334"/>
-    <mergeCell ref="E333:E334"/>
-    <mergeCell ref="F333:I333"/>
-    <mergeCell ref="J333:J334"/>
-    <mergeCell ref="C323:C324"/>
-    <mergeCell ref="D323:D324"/>
-    <mergeCell ref="E323:E324"/>
-    <mergeCell ref="F323:I323"/>
-    <mergeCell ref="J323:J324"/>
-    <mergeCell ref="C362:C363"/>
-    <mergeCell ref="D362:D363"/>
-    <mergeCell ref="E362:E363"/>
-    <mergeCell ref="F362:I362"/>
-    <mergeCell ref="J362:J363"/>
-    <mergeCell ref="C351:C352"/>
-    <mergeCell ref="D351:D352"/>
-    <mergeCell ref="E351:E352"/>
-    <mergeCell ref="F351:I351"/>
-    <mergeCell ref="J351:J352"/>
-    <mergeCell ref="C388:C389"/>
-    <mergeCell ref="D388:D389"/>
-    <mergeCell ref="E388:E389"/>
-    <mergeCell ref="F388:I388"/>
-    <mergeCell ref="J388:J389"/>
-    <mergeCell ref="C376:C377"/>
-    <mergeCell ref="D376:D377"/>
-    <mergeCell ref="E376:E377"/>
-    <mergeCell ref="F376:I376"/>
-    <mergeCell ref="J376:J377"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="D25:D26"/>
     <mergeCell ref="E25:E26"/>
@@ -9252,39 +9220,71 @@
     <mergeCell ref="J25:J26"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="J43:J44"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="J32:J33"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="F55:I55"/>
-    <mergeCell ref="J55:J56"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="D66:D67"/>
-    <mergeCell ref="E66:E67"/>
-    <mergeCell ref="F66:I66"/>
-    <mergeCell ref="J66:J67"/>
-    <mergeCell ref="C99:C100"/>
-    <mergeCell ref="D99:D100"/>
-    <mergeCell ref="E99:E100"/>
-    <mergeCell ref="F99:I99"/>
-    <mergeCell ref="J99:J100"/>
-    <mergeCell ref="D82:D83"/>
-    <mergeCell ref="E82:E83"/>
-    <mergeCell ref="F82:I82"/>
-    <mergeCell ref="J82:J83"/>
-    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="C149:C150"/>
+    <mergeCell ref="D149:D150"/>
+    <mergeCell ref="E149:E150"/>
+    <mergeCell ref="F149:I149"/>
+    <mergeCell ref="J149:J150"/>
+    <mergeCell ref="C175:C176"/>
+    <mergeCell ref="D175:D176"/>
+    <mergeCell ref="E175:E176"/>
+    <mergeCell ref="F175:I175"/>
+    <mergeCell ref="J175:J176"/>
+    <mergeCell ref="C186:C187"/>
+    <mergeCell ref="D186:D187"/>
+    <mergeCell ref="E186:E187"/>
+    <mergeCell ref="F186:I186"/>
+    <mergeCell ref="J186:J187"/>
+    <mergeCell ref="C196:C197"/>
+    <mergeCell ref="D196:D197"/>
+    <mergeCell ref="E196:E197"/>
+    <mergeCell ref="F196:I196"/>
+    <mergeCell ref="J196:J197"/>
+    <mergeCell ref="C206:C207"/>
+    <mergeCell ref="D206:D207"/>
+    <mergeCell ref="E206:E207"/>
+    <mergeCell ref="F206:I206"/>
+    <mergeCell ref="J206:J207"/>
+    <mergeCell ref="C215:C216"/>
+    <mergeCell ref="D215:D216"/>
+    <mergeCell ref="E215:E216"/>
+    <mergeCell ref="F215:I215"/>
+    <mergeCell ref="J215:J216"/>
+    <mergeCell ref="C223:C224"/>
+    <mergeCell ref="D223:D224"/>
+    <mergeCell ref="E223:E224"/>
+    <mergeCell ref="F223:I223"/>
+    <mergeCell ref="J223:J224"/>
+    <mergeCell ref="C232:C233"/>
+    <mergeCell ref="D232:D233"/>
+    <mergeCell ref="E232:E233"/>
+    <mergeCell ref="F232:I232"/>
+    <mergeCell ref="J232:J233"/>
+    <mergeCell ref="C240:C241"/>
+    <mergeCell ref="D240:D241"/>
+    <mergeCell ref="E240:E241"/>
+    <mergeCell ref="F240:I240"/>
+    <mergeCell ref="J240:J241"/>
+    <mergeCell ref="C253:C254"/>
+    <mergeCell ref="D253:D254"/>
+    <mergeCell ref="E253:E254"/>
+    <mergeCell ref="F253:I253"/>
+    <mergeCell ref="J253:J254"/>
+    <mergeCell ref="C282:C283"/>
+    <mergeCell ref="D282:D283"/>
+    <mergeCell ref="E282:E283"/>
+    <mergeCell ref="F282:I282"/>
+    <mergeCell ref="J282:J283"/>
+    <mergeCell ref="C263:C264"/>
+    <mergeCell ref="D263:D264"/>
+    <mergeCell ref="E263:E264"/>
+    <mergeCell ref="F263:I263"/>
+    <mergeCell ref="J263:J264"/>
+    <mergeCell ref="C273:C274"/>
+    <mergeCell ref="D273:D274"/>
+    <mergeCell ref="E273:E274"/>
+    <mergeCell ref="F273:I273"/>
+    <mergeCell ref="J273:J274"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
UI-727: Updated TestPlan to reflect changes on device restrictions
</commit_message>
<xml_diff>
--- a/design/Test Plan/TestPlan.xlsx
+++ b/design/Test Plan/TestPlan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1654" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1657" uniqueCount="469">
   <si>
     <t>Application Name</t>
   </si>
@@ -904,18 +904,6 @@
     <t>The "Restrictions Settings" section containing toggle buttons and a test field will appear</t>
   </si>
   <si>
-    <t>Set some toggle buttons to "Deny"</t>
-  </si>
-  <si>
-    <t>The toggle buttons set to deny will become red</t>
-  </si>
-  <si>
-    <t>Type a valid phone number in the testing field and click on the "Test" button</t>
-  </si>
-  <si>
-    <t>The sentence "The above number matched this rule" will appear next to toggle buttons corresponding to the rules that the phone number matched</t>
-  </si>
-  <si>
     <t>Click on the "Advanced" button, select the "Emergency Caller-ID" option and select a phone number in the dropdown</t>
   </si>
   <si>
@@ -1415,6 +1403,24 @@
   </si>
   <si>
     <t>To upload a new file follow steps from 21B to 21C</t>
+  </si>
+  <si>
+    <t>Set the toggle button for "US Tollfree" to deny, and the one for US DID to allow</t>
+  </si>
+  <si>
+    <t>The Deny ones are displayed in red, the allow ones are green</t>
+  </si>
+  <si>
+    <t>Type in "8003334444" in the testing field and click on the "Test" button</t>
+  </si>
+  <si>
+    <t>A red cross appears next to the US Tollfree line, and a message stating that the call would not be allowed appears in a red box</t>
+  </si>
+  <si>
+    <t>Type in "4153334444" in the testing field and click on the "Test" button</t>
+  </si>
+  <si>
+    <t>A green checkmark appears next to the US DID line, and a message stating that the call would be allowed appears in a green box</t>
   </si>
 </sst>
 </file>
@@ -1674,7 +1680,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1873,6 +1879,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1906,14 +1921,54 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2225,10 +2280,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L392"/>
+  <dimension ref="B2:L393"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A309" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D317" sqref="D317"/>
+    <sheetView tabSelected="1" topLeftCell="A341" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D345" sqref="D345"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2249,51 +2304,51 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="26.45" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="72"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="75"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="76"/>
+      <c r="C3" s="79"/>
       <c r="D3" s="11" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="77" t="s">
+      <c r="B4" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="78"/>
+      <c r="C4" s="81"/>
       <c r="D4" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="79" t="s">
+      <c r="B5" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="80"/>
+      <c r="C5" s="83"/>
       <c r="D5" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="73" t="s">
+      <c r="B6" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="74"/>
+      <c r="C6" s="77"/>
       <c r="D6" s="19"/>
     </row>
     <row r="7" spans="2:12" s="3" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="74"/>
+      <c r="C7" s="77"/>
       <c r="D7" s="23" t="s">
         <v>24</v>
       </c>
@@ -2301,17 +2356,17 @@
       <c r="L7" s="2"/>
     </row>
     <row r="8" spans="2:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="74"/>
+      <c r="C8" s="77"/>
       <c r="D8" s="13"/>
     </row>
     <row r="10" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="56"/>
       <c r="D10" s="56"/>
       <c r="E10" s="59" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="F10" s="56"/>
       <c r="G10" s="56"/>
@@ -2338,7 +2393,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="43" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E13" s="44"/>
       <c r="F13" s="44"/>
@@ -2390,10 +2445,10 @@
         <v>10</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="F16" s="16"/>
       <c r="G16" s="18" t="s">
@@ -2412,10 +2467,10 @@
         <v>11</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="E17" s="27" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="F17" s="28"/>
       <c r="G17" s="29" t="s">
@@ -2434,10 +2489,10 @@
         <v>12</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="21" t="s">
@@ -2456,10 +2511,10 @@
         <v>22</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="E19" s="27" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="F19" s="28"/>
       <c r="G19" s="29" t="s">
@@ -2478,10 +2533,10 @@
         <v>27</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="F20" s="16"/>
       <c r="G20" s="18" t="s">
@@ -2500,10 +2555,10 @@
         <v>28</v>
       </c>
       <c r="D21" s="33" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="E21" s="27" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="F21" s="28"/>
       <c r="G21" s="29" t="s">
@@ -2536,7 +2591,7 @@
         <v>2</v>
       </c>
       <c r="D24" s="43" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="E24" s="44"/>
       <c r="F24" s="44"/>
@@ -2588,10 +2643,10 @@
         <v>10</v>
       </c>
       <c r="D27" s="32" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="F27" s="16"/>
       <c r="G27" s="18" t="s">
@@ -2610,10 +2665,10 @@
         <v>11</v>
       </c>
       <c r="D28" s="33" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E28" s="27" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F28" s="28"/>
       <c r="G28" s="29" t="s">
@@ -2665,12 +2720,12 @@
       <c r="E32" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="F32" s="81" t="s">
+      <c r="F32" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="G32" s="82"/>
-      <c r="H32" s="82"/>
-      <c r="I32" s="83"/>
+      <c r="G32" s="71"/>
+      <c r="H32" s="71"/>
+      <c r="I32" s="72"/>
       <c r="J32" s="68" t="s">
         <v>8</v>
       </c>
@@ -2698,10 +2753,10 @@
         <v>10</v>
       </c>
       <c r="D34" s="32" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="F34" s="16"/>
       <c r="G34" s="18" t="s">
@@ -2720,10 +2775,10 @@
         <v>11</v>
       </c>
       <c r="D35" s="33" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="E35" s="27" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="F35" s="28"/>
       <c r="G35" s="29" t="s">
@@ -2742,7 +2797,7 @@
         <v>12</v>
       </c>
       <c r="D36" s="34" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>206</v>
@@ -2764,10 +2819,10 @@
         <v>22</v>
       </c>
       <c r="D37" s="33" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="E37" s="27" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="F37" s="28"/>
       <c r="G37" s="29" t="s">
@@ -2785,7 +2840,7 @@
       <c r="C39" s="56"/>
       <c r="D39" s="56"/>
       <c r="E39" s="59" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="F39" s="56"/>
       <c r="G39" s="56"/>
@@ -2812,7 +2867,7 @@
         <v>4</v>
       </c>
       <c r="D42" s="43" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="E42" s="44"/>
       <c r="F42" s="44"/>
@@ -2864,10 +2919,10 @@
         <v>10</v>
       </c>
       <c r="D45" s="32" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="F45" s="16"/>
       <c r="G45" s="18" t="s">
@@ -2886,10 +2941,10 @@
         <v>11</v>
       </c>
       <c r="D46" s="33" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="E46" s="27" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="F46" s="28"/>
       <c r="G46" s="29" t="s">
@@ -2908,10 +2963,10 @@
         <v>12</v>
       </c>
       <c r="D47" s="34" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="F47" s="17"/>
       <c r="G47" s="21" t="s">
@@ -2930,10 +2985,10 @@
         <v>22</v>
       </c>
       <c r="D48" s="33" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="E48" s="27" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F48" s="28"/>
       <c r="G48" s="29" t="s">
@@ -2952,10 +3007,10 @@
         <v>27</v>
       </c>
       <c r="D49" s="32" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="F49" s="16"/>
       <c r="G49" s="18" t="s">
@@ -2977,7 +3032,7 @@
         <v>121</v>
       </c>
       <c r="E50" s="27" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="F50" s="28"/>
       <c r="G50" s="29" t="s">
@@ -2996,10 +3051,10 @@
         <v>29</v>
       </c>
       <c r="D51" s="35" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="E51" s="36" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="F51" s="25"/>
       <c r="G51" s="26" t="s">
@@ -3032,7 +3087,7 @@
         <v>5</v>
       </c>
       <c r="D54" s="43" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="E54" s="44"/>
       <c r="F54" s="44"/>
@@ -3084,10 +3139,10 @@
         <v>10</v>
       </c>
       <c r="D57" s="32" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="F57" s="16"/>
       <c r="G57" s="18" t="s">
@@ -3106,10 +3161,10 @@
         <v>11</v>
       </c>
       <c r="D58" s="33" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="E58" s="27" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="F58" s="28"/>
       <c r="G58" s="29" t="s">
@@ -3128,10 +3183,10 @@
         <v>12</v>
       </c>
       <c r="D59" s="34" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="F59" s="17"/>
       <c r="G59" s="21" t="s">
@@ -3150,10 +3205,10 @@
         <v>22</v>
       </c>
       <c r="D60" s="33" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="E60" s="27" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="F60" s="28"/>
       <c r="G60" s="29" t="s">
@@ -3172,10 +3227,10 @@
         <v>27</v>
       </c>
       <c r="D61" s="32" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="F61" s="16"/>
       <c r="G61" s="18" t="s">
@@ -3197,7 +3252,7 @@
         <v>134</v>
       </c>
       <c r="E62" s="27" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="F62" s="28"/>
       <c r="G62" s="29" t="s">
@@ -3230,7 +3285,7 @@
         <v>6</v>
       </c>
       <c r="D65" s="43" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="E65" s="44"/>
       <c r="F65" s="44"/>
@@ -3282,10 +3337,10 @@
         <v>10</v>
       </c>
       <c r="D68" s="32" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="F68" s="16"/>
       <c r="G68" s="18" t="s">
@@ -3304,10 +3359,10 @@
         <v>11</v>
       </c>
       <c r="D69" s="33" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="E69" s="27" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="F69" s="28"/>
       <c r="G69" s="29" t="s">
@@ -3326,10 +3381,10 @@
         <v>12</v>
       </c>
       <c r="D70" s="34" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="F70" s="17"/>
       <c r="G70" s="21" t="s">
@@ -3348,10 +3403,10 @@
         <v>22</v>
       </c>
       <c r="D71" s="33" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="E71" s="27" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="F71" s="28"/>
       <c r="G71" s="29" t="s">
@@ -3370,10 +3425,10 @@
         <v>27</v>
       </c>
       <c r="D72" s="32" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F72" s="16"/>
       <c r="G72" s="18" t="s">
@@ -3392,10 +3447,10 @@
         <v>28</v>
       </c>
       <c r="D73" s="33" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="E73" s="27" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="F73" s="28"/>
       <c r="G73" s="29" t="s">
@@ -3414,10 +3469,10 @@
         <v>29</v>
       </c>
       <c r="D74" s="32" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="F74" s="16"/>
       <c r="G74" s="18" t="s">
@@ -3436,10 +3491,10 @@
         <v>30</v>
       </c>
       <c r="D75" s="33" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="E75" s="27" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="F75" s="28"/>
       <c r="G75" s="29" t="s">
@@ -3458,10 +3513,10 @@
         <v>31</v>
       </c>
       <c r="D76" s="32" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="F76" s="16"/>
       <c r="G76" s="18" t="s">
@@ -3480,10 +3535,10 @@
         <v>32</v>
       </c>
       <c r="D77" s="33" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="E77" s="27" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="F77" s="28"/>
       <c r="G77" s="29" t="s">
@@ -3505,7 +3560,7 @@
         <v>134</v>
       </c>
       <c r="E78" s="7" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="F78" s="17"/>
       <c r="G78" s="21" t="s">
@@ -3538,7 +3593,7 @@
         <v>7</v>
       </c>
       <c r="D81" s="43" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="E81" s="44"/>
       <c r="F81" s="44"/>
@@ -3590,10 +3645,10 @@
         <v>10</v>
       </c>
       <c r="D84" s="32" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="F84" s="16"/>
       <c r="G84" s="18" t="s">
@@ -3612,10 +3667,10 @@
         <v>11</v>
       </c>
       <c r="D85" s="33" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="E85" s="27" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="F85" s="28"/>
       <c r="G85" s="29" t="s">
@@ -3634,10 +3689,10 @@
         <v>12</v>
       </c>
       <c r="D86" s="35" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="E86" s="7" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="F86" s="17"/>
       <c r="G86" s="21" t="s">
@@ -3656,10 +3711,10 @@
         <v>22</v>
       </c>
       <c r="D87" s="33" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="E87" s="27" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="F87" s="28"/>
       <c r="G87" s="29" t="s">
@@ -3678,10 +3733,10 @@
         <v>27</v>
       </c>
       <c r="D88" s="32" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="F88" s="16"/>
       <c r="G88" s="18" t="s">
@@ -3700,10 +3755,10 @@
         <v>28</v>
       </c>
       <c r="D89" s="33" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="E89" s="27" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="F89" s="28"/>
       <c r="G89" s="29" t="s">
@@ -3722,10 +3777,10 @@
         <v>29</v>
       </c>
       <c r="D90" s="32" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="F90" s="16"/>
       <c r="G90" s="18" t="s">
@@ -3744,10 +3799,10 @@
         <v>30</v>
       </c>
       <c r="D91" s="33" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="E91" s="27" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="F91" s="28"/>
       <c r="G91" s="29" t="s">
@@ -3766,10 +3821,10 @@
         <v>31</v>
       </c>
       <c r="D92" s="32" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="E92" s="9" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="F92" s="16"/>
       <c r="G92" s="18" t="s">
@@ -3788,10 +3843,10 @@
         <v>32</v>
       </c>
       <c r="D93" s="33" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="E93" s="27" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="F93" s="28"/>
       <c r="G93" s="29" t="s">
@@ -3810,10 +3865,10 @@
         <v>33</v>
       </c>
       <c r="D94" s="34" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="F94" s="17"/>
       <c r="G94" s="21" t="s">
@@ -3835,7 +3890,7 @@
         <v>134</v>
       </c>
       <c r="E95" s="27" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="F95" s="28"/>
       <c r="G95" s="29" t="s">
@@ -3868,7 +3923,7 @@
         <v>8</v>
       </c>
       <c r="D98" s="43" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="E98" s="44"/>
       <c r="F98" s="44"/>
@@ -3920,10 +3975,10 @@
         <v>10</v>
       </c>
       <c r="D101" s="32" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E101" s="9" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F101" s="16"/>
       <c r="G101" s="18" t="s">
@@ -3942,10 +3997,10 @@
         <v>11</v>
       </c>
       <c r="D102" s="33" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="E102" s="27" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="F102" s="28"/>
       <c r="G102" s="29" t="s">
@@ -3964,10 +4019,10 @@
         <v>12</v>
       </c>
       <c r="D103" s="34" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="F103" s="17"/>
       <c r="G103" s="21" t="s">
@@ -3986,10 +4041,10 @@
         <v>22</v>
       </c>
       <c r="D104" s="33" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="E104" s="27" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="F104" s="28"/>
       <c r="G104" s="29" t="s">
@@ -4007,7 +4062,7 @@
       <c r="C106" s="56"/>
       <c r="D106" s="56"/>
       <c r="E106" s="59" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="F106" s="56"/>
       <c r="G106" s="56"/>
@@ -6901,7 +6956,7 @@
       <c r="C269" s="56"/>
       <c r="D269" s="56"/>
       <c r="E269" s="59" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="F269" s="56"/>
       <c r="G269" s="56"/>
@@ -7772,7 +7827,7 @@
         <v>11</v>
       </c>
       <c r="D317" s="33" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="E317" s="27" t="s">
         <v>271</v>
@@ -7969,7 +8024,7 @@
       <c r="C329" s="56"/>
       <c r="D329" s="56"/>
       <c r="E329" s="59" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="F329" s="56"/>
       <c r="G329" s="56"/>
@@ -8161,7 +8216,7 @@
         <v>293</v>
       </c>
       <c r="E340" s="27" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="F340" s="28"/>
       <c r="G340" s="29" t="s">
@@ -8197,15 +8252,15 @@
       </c>
       <c r="J341" s="10"/>
     </row>
-    <row r="342" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="342" spans="3:10" ht="30" x14ac:dyDescent="0.25">
       <c r="C342" s="39" t="s">
         <v>30</v>
       </c>
       <c r="D342" s="33" t="s">
-        <v>296</v>
+        <v>463</v>
       </c>
       <c r="E342" s="27" t="s">
-        <v>297</v>
+        <v>464</v>
       </c>
       <c r="F342" s="28"/>
       <c r="G342" s="29" t="s">
@@ -8219,15 +8274,15 @@
       </c>
       <c r="J342" s="31"/>
     </row>
-    <row r="343" spans="3:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="343" spans="3:10" ht="45" x14ac:dyDescent="0.25">
       <c r="C343" s="38" t="s">
         <v>31</v>
       </c>
       <c r="D343" s="32" t="s">
-        <v>298</v>
+        <v>465</v>
       </c>
       <c r="E343" s="9" t="s">
-        <v>299</v>
+        <v>466</v>
       </c>
       <c r="F343" s="16"/>
       <c r="G343" s="18" t="s">
@@ -8242,80 +8297,74 @@
       <c r="J343" s="10"/>
     </row>
     <row r="344" spans="3:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="C344" s="39" t="s">
+      <c r="C344" s="84" t="s">
         <v>32</v>
       </c>
-      <c r="D344" s="33" t="s">
-        <v>300</v>
-      </c>
-      <c r="E344" s="27" t="s">
-        <v>301</v>
-      </c>
-      <c r="F344" s="28"/>
-      <c r="G344" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="H344" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I344" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="J344" s="31"/>
-    </row>
-    <row r="345" spans="3:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C345" s="40" t="s">
+      <c r="D344" s="85" t="s">
+        <v>467</v>
+      </c>
+      <c r="E344" s="86" t="s">
+        <v>468</v>
+      </c>
+      <c r="F344" s="87"/>
+      <c r="G344" s="88"/>
+      <c r="H344" s="88"/>
+      <c r="I344" s="89"/>
+      <c r="J344" s="90"/>
+    </row>
+    <row r="345" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="C345" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="D345" s="34" t="s">
-        <v>302</v>
-      </c>
-      <c r="E345" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="F345" s="17"/>
-      <c r="G345" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="H345" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I345" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="J345" s="8"/>
-    </row>
-    <row r="346" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C346" s="39" t="s">
+      <c r="D345" s="53" t="s">
+        <v>296</v>
+      </c>
+      <c r="E345" s="54" t="s">
+        <v>297</v>
+      </c>
+      <c r="F345" s="25"/>
+      <c r="G345" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="H345" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="I345" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="J345" s="55"/>
+    </row>
+    <row r="346" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="C346" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="D346" s="33" t="s">
-        <v>304</v>
-      </c>
-      <c r="E346" s="27" t="s">
-        <v>305</v>
-      </c>
-      <c r="F346" s="28"/>
-      <c r="G346" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="H346" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I346" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="J346" s="31"/>
-    </row>
-    <row r="347" spans="3:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="D346" s="92" t="s">
+        <v>298</v>
+      </c>
+      <c r="E346" s="93" t="s">
+        <v>299</v>
+      </c>
+      <c r="F346" s="94"/>
+      <c r="G346" s="95" t="s">
+        <v>17</v>
+      </c>
+      <c r="H346" s="95" t="s">
+        <v>17</v>
+      </c>
+      <c r="I346" s="96" t="s">
+        <v>17</v>
+      </c>
+      <c r="J346" s="97"/>
+    </row>
+    <row r="347" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C347" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="D347" s="35" t="s">
-        <v>306</v>
-      </c>
-      <c r="E347" s="36" t="s">
-        <v>317</v>
+      <c r="D347" s="53" t="s">
+        <v>300</v>
+      </c>
+      <c r="E347" s="54" t="s">
+        <v>301</v>
       </c>
       <c r="F347" s="25"/>
       <c r="G347" s="26" t="s">
@@ -8327,875 +8376,879 @@
       <c r="I347" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="J347" s="6"/>
-    </row>
-    <row r="349" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C349" s="24" t="s">
+      <c r="J347" s="55"/>
+    </row>
+    <row r="348" spans="3:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="C348" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="D348" s="98" t="s">
+        <v>302</v>
+      </c>
+      <c r="E348" s="99" t="s">
+        <v>313</v>
+      </c>
+      <c r="F348" s="28"/>
+      <c r="G348" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="H348" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I348" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="J348" s="100"/>
+    </row>
+    <row r="350" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C350" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="D349" s="4" t="s">
+      <c r="D350" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E349" s="4"/>
-      <c r="F349" s="4"/>
-      <c r="G349" s="4"/>
-      <c r="H349" s="4"/>
-      <c r="I349" s="4"/>
-      <c r="J349" s="5"/>
-    </row>
-    <row r="350" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C350" s="42">
+      <c r="E350" s="4"/>
+      <c r="F350" s="4"/>
+      <c r="G350" s="4"/>
+      <c r="H350" s="4"/>
+      <c r="I350" s="4"/>
+      <c r="J350" s="5"/>
+    </row>
+    <row r="351" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C351" s="42">
         <v>30</v>
       </c>
-      <c r="D350" s="43" t="s">
+      <c r="D351" s="43" t="s">
+        <v>303</v>
+      </c>
+      <c r="E351" s="44"/>
+      <c r="F351" s="44"/>
+      <c r="G351" s="44"/>
+      <c r="H351" s="44"/>
+      <c r="I351" s="44"/>
+      <c r="J351" s="45"/>
+    </row>
+    <row r="352" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C352" s="60" t="s">
+        <v>9</v>
+      </c>
+      <c r="D352" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="E352" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="F352" s="66" t="s">
+        <v>14</v>
+      </c>
+      <c r="G352" s="67"/>
+      <c r="H352" s="67"/>
+      <c r="I352" s="64"/>
+      <c r="J352" s="68" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="353" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="C353" s="61"/>
+      <c r="D353" s="63"/>
+      <c r="E353" s="65"/>
+      <c r="F353" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G353" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H353" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I353" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="J353" s="69"/>
+    </row>
+    <row r="354" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="C354" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="D354" s="32" t="s">
+        <v>304</v>
+      </c>
+      <c r="E354" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="F354" s="16"/>
+      <c r="G354" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H354" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="I354" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J354" s="10"/>
+    </row>
+    <row r="355" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C355" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D355" s="33" t="s">
+        <v>459</v>
+      </c>
+      <c r="E355" s="27" t="s">
+        <v>461</v>
+      </c>
+      <c r="F355" s="28"/>
+      <c r="G355" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="H355" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I355" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="J355" s="31"/>
+    </row>
+    <row r="356" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="C356" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D356" s="34" t="s">
+        <v>306</v>
+      </c>
+      <c r="E356" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="E350" s="44"/>
-      <c r="F350" s="44"/>
-      <c r="G350" s="44"/>
-      <c r="H350" s="44"/>
-      <c r="I350" s="44"/>
-      <c r="J350" s="45"/>
-    </row>
-    <row r="351" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C351" s="60" t="s">
+      <c r="F356" s="17"/>
+      <c r="G356" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H356" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="I356" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="J356" s="8"/>
+    </row>
+    <row r="357" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C357" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="D357" s="33" t="s">
+        <v>308</v>
+      </c>
+      <c r="E357" s="27" t="s">
+        <v>461</v>
+      </c>
+      <c r="F357" s="28"/>
+      <c r="G357" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="H357" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I357" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="J357" s="31"/>
+    </row>
+    <row r="358" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="C358" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D358" s="32" t="s">
+        <v>309</v>
+      </c>
+      <c r="E358" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="F358" s="16"/>
+      <c r="G358" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H358" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="I358" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J358" s="10"/>
+    </row>
+    <row r="359" spans="3:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="C359" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="D359" s="33" t="s">
+        <v>311</v>
+      </c>
+      <c r="E359" s="27" t="s">
+        <v>313</v>
+      </c>
+      <c r="F359" s="28"/>
+      <c r="G359" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="H359" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I359" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="J359" s="31"/>
+    </row>
+    <row r="361" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C361" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D361" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E361" s="4"/>
+      <c r="F361" s="4"/>
+      <c r="G361" s="4"/>
+      <c r="H361" s="4"/>
+      <c r="I361" s="4"/>
+      <c r="J361" s="5"/>
+    </row>
+    <row r="362" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C362" s="42">
+        <v>31</v>
+      </c>
+      <c r="D362" s="43" t="s">
+        <v>312</v>
+      </c>
+      <c r="E362" s="44"/>
+      <c r="F362" s="44"/>
+      <c r="G362" s="44"/>
+      <c r="H362" s="44"/>
+      <c r="I362" s="44"/>
+      <c r="J362" s="45"/>
+    </row>
+    <row r="363" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C363" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="D351" s="62" t="s">
+      <c r="D363" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="E351" s="64" t="s">
+      <c r="E363" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="F351" s="66" t="s">
+      <c r="F363" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="G351" s="67"/>
-      <c r="H351" s="67"/>
-      <c r="I351" s="64"/>
-      <c r="J351" s="68" t="s">
+      <c r="G363" s="67"/>
+      <c r="H363" s="67"/>
+      <c r="I363" s="64"/>
+      <c r="J363" s="68" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="352" spans="3:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C352" s="61"/>
-      <c r="D352" s="63"/>
-      <c r="E352" s="65"/>
-      <c r="F352" s="14" t="s">
+    <row r="364" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="C364" s="61"/>
+      <c r="D364" s="63"/>
+      <c r="E364" s="65"/>
+      <c r="F364" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G352" s="15" t="s">
+      <c r="G364" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="H352" s="14" t="s">
+      <c r="H364" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="I352" s="14" t="s">
+      <c r="I364" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J352" s="69"/>
-    </row>
-    <row r="353" spans="3:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C353" s="38" t="s">
+      <c r="J364" s="69"/>
+    </row>
+    <row r="365" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="C365" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="D353" s="32" t="s">
-        <v>308</v>
-      </c>
-      <c r="E353" s="9" t="s">
-        <v>309</v>
-      </c>
-      <c r="F353" s="16"/>
-      <c r="G353" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="H353" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="I353" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="J353" s="10"/>
-    </row>
-    <row r="354" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C354" s="39" t="s">
+      <c r="D365" s="32" t="s">
+        <v>317</v>
+      </c>
+      <c r="E365" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="F365" s="16"/>
+      <c r="G365" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H365" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="I365" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J365" s="10"/>
+    </row>
+    <row r="366" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="C366" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D354" s="33" t="s">
-        <v>463</v>
-      </c>
-      <c r="E354" s="27" t="s">
-        <v>465</v>
-      </c>
-      <c r="F354" s="28"/>
-      <c r="G354" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="H354" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I354" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="J354" s="31"/>
-    </row>
-    <row r="355" spans="3:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C355" s="40" t="s">
+      <c r="D366" s="33" t="s">
+        <v>319</v>
+      </c>
+      <c r="E366" s="27" t="s">
+        <v>320</v>
+      </c>
+      <c r="F366" s="28"/>
+      <c r="G366" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="H366" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I366" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="J366" s="31"/>
+    </row>
+    <row r="367" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="C367" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="D355" s="34" t="s">
-        <v>310</v>
-      </c>
-      <c r="E355" s="7" t="s">
-        <v>311</v>
-      </c>
-      <c r="F355" s="17"/>
-      <c r="G355" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="H355" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I355" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="J355" s="8"/>
-    </row>
-    <row r="356" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C356" s="39" t="s">
+      <c r="D367" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="E367" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="F367" s="17"/>
+      <c r="G367" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H367" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="I367" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="J367" s="8"/>
+    </row>
+    <row r="368" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="C368" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="D356" s="33" t="s">
-        <v>312</v>
-      </c>
-      <c r="E356" s="27" t="s">
-        <v>465</v>
-      </c>
-      <c r="F356" s="28"/>
-      <c r="G356" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="H356" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I356" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="J356" s="31"/>
-    </row>
-    <row r="357" spans="3:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C357" s="38" t="s">
+      <c r="D368" s="33" t="s">
+        <v>322</v>
+      </c>
+      <c r="E368" s="27" t="s">
+        <v>323</v>
+      </c>
+      <c r="F368" s="28"/>
+      <c r="G368" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="H368" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I368" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="J368" s="31"/>
+    </row>
+    <row r="369" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="C369" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="D357" s="32" t="s">
-        <v>313</v>
-      </c>
-      <c r="E357" s="9" t="s">
-        <v>314</v>
-      </c>
-      <c r="F357" s="16"/>
-      <c r="G357" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="H357" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="I357" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="J357" s="10"/>
-    </row>
-    <row r="358" spans="3:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="C358" s="39" t="s">
+      <c r="D369" s="32" t="s">
+        <v>324</v>
+      </c>
+      <c r="E369" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="F369" s="16"/>
+      <c r="G369" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H369" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="I369" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J369" s="10"/>
+    </row>
+    <row r="370" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="C370" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="D358" s="33" t="s">
-        <v>315</v>
-      </c>
-      <c r="E358" s="27" t="s">
-        <v>317</v>
-      </c>
-      <c r="F358" s="28"/>
-      <c r="G358" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="H358" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I358" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="J358" s="31"/>
-    </row>
-    <row r="360" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C360" s="24" t="s">
+      <c r="D370" s="33" t="s">
+        <v>326</v>
+      </c>
+      <c r="E370" s="27" t="s">
+        <v>327</v>
+      </c>
+      <c r="F370" s="28"/>
+      <c r="G370" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="H370" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I370" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="J370" s="31"/>
+    </row>
+    <row r="371" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="C371" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="D371" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="E371" s="36" t="s">
+        <v>328</v>
+      </c>
+      <c r="F371" s="25"/>
+      <c r="G371" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="H371" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="I371" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="J371" s="6"/>
+    </row>
+    <row r="373" spans="3:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C373" s="56"/>
+      <c r="D373" s="56"/>
+      <c r="E373" s="59" t="s">
+        <v>329</v>
+      </c>
+      <c r="F373" s="56"/>
+      <c r="G373" s="56"/>
+      <c r="H373" s="57"/>
+      <c r="I373" s="57"/>
+      <c r="J373" s="58"/>
+    </row>
+    <row r="375" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C375" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="D360" s="4" t="s">
+      <c r="D375" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E360" s="4"/>
-      <c r="F360" s="4"/>
-      <c r="G360" s="4"/>
-      <c r="H360" s="4"/>
-      <c r="I360" s="4"/>
-      <c r="J360" s="5"/>
-    </row>
-    <row r="361" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C361" s="42">
-        <v>31</v>
-      </c>
-      <c r="D361" s="43" t="s">
-        <v>316</v>
-      </c>
-      <c r="E361" s="44"/>
-      <c r="F361" s="44"/>
-      <c r="G361" s="44"/>
-      <c r="H361" s="44"/>
-      <c r="I361" s="44"/>
-      <c r="J361" s="45"/>
-    </row>
-    <row r="362" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C362" s="60" t="s">
+      <c r="E375" s="4"/>
+      <c r="F375" s="4"/>
+      <c r="G375" s="4"/>
+      <c r="H375" s="4"/>
+      <c r="I375" s="4"/>
+      <c r="J375" s="5"/>
+    </row>
+    <row r="376" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C376" s="42">
+        <v>32</v>
+      </c>
+      <c r="D376" s="43" t="s">
+        <v>332</v>
+      </c>
+      <c r="E376" s="44"/>
+      <c r="F376" s="44"/>
+      <c r="G376" s="44"/>
+      <c r="H376" s="44"/>
+      <c r="I376" s="44"/>
+      <c r="J376" s="45"/>
+    </row>
+    <row r="377" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C377" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="D362" s="62" t="s">
+      <c r="D377" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="E362" s="64" t="s">
+      <c r="E377" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="F362" s="66" t="s">
+      <c r="F377" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="G362" s="67"/>
-      <c r="H362" s="67"/>
-      <c r="I362" s="64"/>
-      <c r="J362" s="68" t="s">
+      <c r="G377" s="67"/>
+      <c r="H377" s="67"/>
+      <c r="I377" s="64"/>
+      <c r="J377" s="68" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="363" spans="3:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C363" s="61"/>
-      <c r="D363" s="63"/>
-      <c r="E363" s="65"/>
-      <c r="F363" s="14" t="s">
+    <row r="378" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="C378" s="61"/>
+      <c r="D378" s="63"/>
+      <c r="E378" s="65"/>
+      <c r="F378" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G363" s="15" t="s">
+      <c r="G378" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="H363" s="14" t="s">
+      <c r="H378" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="I363" s="14" t="s">
+      <c r="I378" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J363" s="69"/>
-    </row>
-    <row r="364" spans="3:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="C364" s="38" t="s">
+      <c r="J378" s="69"/>
+    </row>
+    <row r="379" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="C379" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="D364" s="32" t="s">
-        <v>321</v>
-      </c>
-      <c r="E364" s="9" t="s">
-        <v>322</v>
-      </c>
-      <c r="F364" s="16"/>
-      <c r="G364" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="H364" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="I364" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="J364" s="10"/>
-    </row>
-    <row r="365" spans="3:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C365" s="39" t="s">
+      <c r="D379" s="32" t="s">
+        <v>330</v>
+      </c>
+      <c r="E379" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="F379" s="16"/>
+      <c r="G379" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H379" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="I379" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J379" s="10"/>
+    </row>
+    <row r="380" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="C380" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D365" s="33" t="s">
-        <v>323</v>
-      </c>
-      <c r="E365" s="27" t="s">
-        <v>324</v>
-      </c>
-      <c r="F365" s="28"/>
-      <c r="G365" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="H365" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I365" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="J365" s="31"/>
-    </row>
-    <row r="366" spans="3:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C366" s="40" t="s">
+      <c r="D380" s="33" t="s">
+        <v>334</v>
+      </c>
+      <c r="E380" s="27" t="s">
+        <v>335</v>
+      </c>
+      <c r="F380" s="28"/>
+      <c r="G380" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="H380" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I380" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="J380" s="31"/>
+    </row>
+    <row r="381" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="C381" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="D366" s="34" t="s">
-        <v>134</v>
-      </c>
-      <c r="E366" s="7" t="s">
-        <v>325</v>
-      </c>
-      <c r="F366" s="17"/>
-      <c r="G366" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="H366" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I366" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="J366" s="8"/>
-    </row>
-    <row r="367" spans="3:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="C367" s="39" t="s">
+      <c r="D381" s="34" t="s">
+        <v>336</v>
+      </c>
+      <c r="E381" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="F381" s="17"/>
+      <c r="G381" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H381" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="I381" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="J381" s="8"/>
+    </row>
+    <row r="382" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="C382" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="D367" s="33" t="s">
-        <v>326</v>
-      </c>
-      <c r="E367" s="27" t="s">
-        <v>327</v>
-      </c>
-      <c r="F367" s="28"/>
-      <c r="G367" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="H367" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I367" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="J367" s="31"/>
-    </row>
-    <row r="368" spans="3:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="C368" s="38" t="s">
+      <c r="D382" s="33" t="s">
+        <v>338</v>
+      </c>
+      <c r="E382" s="27" t="s">
+        <v>339</v>
+      </c>
+      <c r="F382" s="28"/>
+      <c r="G382" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="H382" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I382" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="J382" s="31"/>
+    </row>
+    <row r="383" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="C383" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="D368" s="32" t="s">
-        <v>328</v>
-      </c>
-      <c r="E368" s="9" t="s">
-        <v>329</v>
-      </c>
-      <c r="F368" s="16"/>
-      <c r="G368" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="H368" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="I368" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="J368" s="10"/>
-    </row>
-    <row r="369" spans="3:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="C369" s="39" t="s">
+      <c r="D383" s="32" t="s">
+        <v>340</v>
+      </c>
+      <c r="E383" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="F383" s="16"/>
+      <c r="G383" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H383" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="I383" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J383" s="10"/>
+    </row>
+    <row r="384" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="C384" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="D369" s="33" t="s">
-        <v>330</v>
-      </c>
-      <c r="E369" s="27" t="s">
-        <v>331</v>
-      </c>
-      <c r="F369" s="28"/>
-      <c r="G369" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="H369" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I369" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="J369" s="31"/>
-    </row>
-    <row r="370" spans="3:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="C370" s="41" t="s">
+      <c r="D384" s="33" t="s">
+        <v>342</v>
+      </c>
+      <c r="E384" s="27" t="s">
+        <v>343</v>
+      </c>
+      <c r="F384" s="28"/>
+      <c r="G384" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="H384" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I384" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="J384" s="31"/>
+    </row>
+    <row r="385" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="C385" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="D370" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="E370" s="36" t="s">
-        <v>332</v>
-      </c>
-      <c r="F370" s="25"/>
-      <c r="G370" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="H370" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="I370" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="J370" s="6"/>
-    </row>
-    <row r="372" spans="3:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C372" s="56"/>
-      <c r="D372" s="56"/>
-      <c r="E372" s="59" t="s">
+      <c r="D385" s="35" t="s">
+        <v>344</v>
+      </c>
+      <c r="E385" s="36" t="s">
+        <v>345</v>
+      </c>
+      <c r="F385" s="25"/>
+      <c r="G385" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="H385" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="I385" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="J385" s="6"/>
+    </row>
+    <row r="387" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C387" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D387" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E387" s="4"/>
+      <c r="F387" s="4"/>
+      <c r="G387" s="4"/>
+      <c r="H387" s="4"/>
+      <c r="I387" s="4"/>
+      <c r="J387" s="5"/>
+    </row>
+    <row r="388" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C388" s="42">
+        <v>33</v>
+      </c>
+      <c r="D388" s="43" t="s">
         <v>333</v>
       </c>
-      <c r="F372" s="56"/>
-      <c r="G372" s="56"/>
-      <c r="H372" s="57"/>
-      <c r="I372" s="57"/>
-      <c r="J372" s="58"/>
-    </row>
-    <row r="374" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C374" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D374" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E374" s="4"/>
-      <c r="F374" s="4"/>
-      <c r="G374" s="4"/>
-      <c r="H374" s="4"/>
-      <c r="I374" s="4"/>
-      <c r="J374" s="5"/>
-    </row>
-    <row r="375" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C375" s="42">
-        <v>32</v>
-      </c>
-      <c r="D375" s="43" t="s">
-        <v>336</v>
-      </c>
-      <c r="E375" s="44"/>
-      <c r="F375" s="44"/>
-      <c r="G375" s="44"/>
-      <c r="H375" s="44"/>
-      <c r="I375" s="44"/>
-      <c r="J375" s="45"/>
-    </row>
-    <row r="376" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C376" s="60" t="s">
+      <c r="E388" s="44"/>
+      <c r="F388" s="44"/>
+      <c r="G388" s="44"/>
+      <c r="H388" s="44"/>
+      <c r="I388" s="44"/>
+      <c r="J388" s="45"/>
+    </row>
+    <row r="389" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C389" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="D376" s="62" t="s">
+      <c r="D389" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="E376" s="64" t="s">
+      <c r="E389" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="F376" s="66" t="s">
+      <c r="F389" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="G376" s="67"/>
-      <c r="H376" s="67"/>
-      <c r="I376" s="64"/>
-      <c r="J376" s="68" t="s">
+      <c r="G389" s="67"/>
+      <c r="H389" s="67"/>
+      <c r="I389" s="64"/>
+      <c r="J389" s="68" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="377" spans="3:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C377" s="61"/>
-      <c r="D377" s="63"/>
-      <c r="E377" s="65"/>
-      <c r="F377" s="14" t="s">
+    <row r="390" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="C390" s="61"/>
+      <c r="D390" s="63"/>
+      <c r="E390" s="65"/>
+      <c r="F390" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G377" s="15" t="s">
+      <c r="G390" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="H377" s="14" t="s">
+      <c r="H390" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="I377" s="14" t="s">
+      <c r="I390" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J377" s="69"/>
-    </row>
-    <row r="378" spans="3:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C378" s="38" t="s">
+      <c r="J390" s="69"/>
+    </row>
+    <row r="391" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="C391" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="D378" s="32" t="s">
-        <v>334</v>
-      </c>
-      <c r="E378" s="9" t="s">
-        <v>335</v>
-      </c>
-      <c r="F378" s="16"/>
-      <c r="G378" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="H378" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="I378" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="J378" s="10"/>
-    </row>
-    <row r="379" spans="3:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="C379" s="39" t="s">
+      <c r="D391" s="32" t="s">
+        <v>347</v>
+      </c>
+      <c r="E391" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="F391" s="16"/>
+      <c r="G391" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H391" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="I391" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J391" s="10"/>
+    </row>
+    <row r="392" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="C392" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D379" s="33" t="s">
-        <v>338</v>
-      </c>
-      <c r="E379" s="27" t="s">
-        <v>339</v>
-      </c>
-      <c r="F379" s="28"/>
-      <c r="G379" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="H379" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I379" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="J379" s="31"/>
-    </row>
-    <row r="380" spans="3:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C380" s="40" t="s">
+      <c r="D392" s="33" t="s">
+        <v>350</v>
+      </c>
+      <c r="E392" s="27" t="s">
+        <v>349</v>
+      </c>
+      <c r="F392" s="28"/>
+      <c r="G392" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="H392" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I392" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="J392" s="31"/>
+    </row>
+    <row r="393" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="C393" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="D380" s="34" t="s">
-        <v>340</v>
-      </c>
-      <c r="E380" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="F380" s="17"/>
-      <c r="G380" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="H380" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I380" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="J380" s="8"/>
-    </row>
-    <row r="381" spans="3:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="C381" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="D381" s="33" t="s">
-        <v>342</v>
-      </c>
-      <c r="E381" s="27" t="s">
-        <v>343</v>
-      </c>
-      <c r="F381" s="28"/>
-      <c r="G381" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="H381" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I381" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="J381" s="31"/>
-    </row>
-    <row r="382" spans="3:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="C382" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="D382" s="32" t="s">
-        <v>344</v>
-      </c>
-      <c r="E382" s="9" t="s">
-        <v>345</v>
-      </c>
-      <c r="F382" s="16"/>
-      <c r="G382" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="H382" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="I382" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="J382" s="10"/>
-    </row>
-    <row r="383" spans="3:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C383" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="D383" s="33" t="s">
-        <v>346</v>
-      </c>
-      <c r="E383" s="27" t="s">
-        <v>347</v>
-      </c>
-      <c r="F383" s="28"/>
-      <c r="G383" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="H383" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I383" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="J383" s="31"/>
-    </row>
-    <row r="384" spans="3:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C384" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="D384" s="35" t="s">
-        <v>348</v>
-      </c>
-      <c r="E384" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="F384" s="25"/>
-      <c r="G384" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="H384" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="I384" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="J384" s="6"/>
-    </row>
-    <row r="386" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C386" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D386" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E386" s="4"/>
-      <c r="F386" s="4"/>
-      <c r="G386" s="4"/>
-      <c r="H386" s="4"/>
-      <c r="I386" s="4"/>
-      <c r="J386" s="5"/>
-    </row>
-    <row r="387" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C387" s="42">
-        <v>33</v>
-      </c>
-      <c r="D387" s="43" t="s">
-        <v>337</v>
-      </c>
-      <c r="E387" s="44"/>
-      <c r="F387" s="44"/>
-      <c r="G387" s="44"/>
-      <c r="H387" s="44"/>
-      <c r="I387" s="44"/>
-      <c r="J387" s="45"/>
-    </row>
-    <row r="388" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C388" s="60" t="s">
-        <v>9</v>
-      </c>
-      <c r="D388" s="62" t="s">
-        <v>6</v>
-      </c>
-      <c r="E388" s="64" t="s">
-        <v>7</v>
-      </c>
-      <c r="F388" s="66" t="s">
-        <v>14</v>
-      </c>
-      <c r="G388" s="67"/>
-      <c r="H388" s="67"/>
-      <c r="I388" s="64"/>
-      <c r="J388" s="68" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="389" spans="3:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C389" s="61"/>
-      <c r="D389" s="63"/>
-      <c r="E389" s="65"/>
-      <c r="F389" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G389" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H389" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I389" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="J389" s="69"/>
-    </row>
-    <row r="390" spans="3:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C390" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="D390" s="32" t="s">
+      <c r="D393" s="34" t="s">
         <v>351</v>
       </c>
-      <c r="E390" s="9" t="s">
+      <c r="E393" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="F390" s="16"/>
-      <c r="G390" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="H390" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="I390" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="J390" s="10"/>
-    </row>
-    <row r="391" spans="3:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="C391" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="D391" s="33" t="s">
-        <v>354</v>
-      </c>
-      <c r="E391" s="27" t="s">
-        <v>353</v>
-      </c>
-      <c r="F391" s="28"/>
-      <c r="G391" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="H391" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I391" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="J391" s="31"/>
-    </row>
-    <row r="392" spans="3:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="C392" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="D392" s="34" t="s">
-        <v>355</v>
-      </c>
-      <c r="E392" s="7" t="s">
-        <v>356</v>
-      </c>
-      <c r="F392" s="17"/>
-      <c r="G392" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="H392" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I392" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="J392" s="8"/>
+      <c r="F393" s="17"/>
+      <c r="G393" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H393" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="I393" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="J393" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="172">
-    <mergeCell ref="C99:C100"/>
-    <mergeCell ref="D99:D100"/>
-    <mergeCell ref="E99:E100"/>
-    <mergeCell ref="F99:I99"/>
-    <mergeCell ref="J99:J100"/>
-    <mergeCell ref="D82:D83"/>
-    <mergeCell ref="E82:E83"/>
-    <mergeCell ref="F82:I82"/>
-    <mergeCell ref="J82:J83"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="F55:I55"/>
-    <mergeCell ref="J55:J56"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="D66:D67"/>
-    <mergeCell ref="E66:E67"/>
-    <mergeCell ref="F66:I66"/>
-    <mergeCell ref="J66:J67"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="J43:J44"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="J32:J33"/>
-    <mergeCell ref="C388:C389"/>
-    <mergeCell ref="D388:D389"/>
-    <mergeCell ref="E388:E389"/>
-    <mergeCell ref="F388:I388"/>
-    <mergeCell ref="J388:J389"/>
-    <mergeCell ref="C376:C377"/>
-    <mergeCell ref="D376:D377"/>
-    <mergeCell ref="E376:E377"/>
-    <mergeCell ref="F376:I376"/>
-    <mergeCell ref="J376:J377"/>
-    <mergeCell ref="C362:C363"/>
-    <mergeCell ref="D362:D363"/>
-    <mergeCell ref="E362:E363"/>
-    <mergeCell ref="F362:I362"/>
-    <mergeCell ref="J362:J363"/>
-    <mergeCell ref="C351:C352"/>
-    <mergeCell ref="D351:D352"/>
-    <mergeCell ref="E351:E352"/>
-    <mergeCell ref="F351:I351"/>
-    <mergeCell ref="J351:J352"/>
-    <mergeCell ref="C333:C334"/>
-    <mergeCell ref="D333:D334"/>
-    <mergeCell ref="E333:E334"/>
-    <mergeCell ref="F333:I333"/>
-    <mergeCell ref="J333:J334"/>
-    <mergeCell ref="C323:C324"/>
-    <mergeCell ref="D323:D324"/>
-    <mergeCell ref="E323:E324"/>
-    <mergeCell ref="F323:I323"/>
-    <mergeCell ref="J323:J324"/>
-    <mergeCell ref="C314:C315"/>
-    <mergeCell ref="D314:D315"/>
-    <mergeCell ref="E314:E315"/>
-    <mergeCell ref="F314:I314"/>
-    <mergeCell ref="J314:J315"/>
-    <mergeCell ref="C306:C307"/>
-    <mergeCell ref="D306:D307"/>
-    <mergeCell ref="E306:E307"/>
-    <mergeCell ref="F306:I306"/>
-    <mergeCell ref="J306:J307"/>
-    <mergeCell ref="C139:C140"/>
-    <mergeCell ref="D139:D140"/>
-    <mergeCell ref="E139:E140"/>
-    <mergeCell ref="F139:I139"/>
-    <mergeCell ref="J139:J140"/>
-    <mergeCell ref="C131:C132"/>
-    <mergeCell ref="D131:D132"/>
-    <mergeCell ref="E131:E132"/>
-    <mergeCell ref="F131:I131"/>
-    <mergeCell ref="J131:J132"/>
+    <mergeCell ref="C282:C283"/>
+    <mergeCell ref="D282:D283"/>
+    <mergeCell ref="E282:E283"/>
+    <mergeCell ref="F282:I282"/>
+    <mergeCell ref="J282:J283"/>
+    <mergeCell ref="C263:C264"/>
+    <mergeCell ref="D263:D264"/>
+    <mergeCell ref="E263:E264"/>
+    <mergeCell ref="F263:I263"/>
+    <mergeCell ref="J263:J264"/>
+    <mergeCell ref="C273:C274"/>
+    <mergeCell ref="D273:D274"/>
+    <mergeCell ref="E273:E274"/>
+    <mergeCell ref="F273:I273"/>
+    <mergeCell ref="J273:J274"/>
+    <mergeCell ref="C240:C241"/>
+    <mergeCell ref="D240:D241"/>
+    <mergeCell ref="E240:E241"/>
+    <mergeCell ref="F240:I240"/>
+    <mergeCell ref="J240:J241"/>
+    <mergeCell ref="C253:C254"/>
+    <mergeCell ref="D253:D254"/>
+    <mergeCell ref="E253:E254"/>
+    <mergeCell ref="F253:I253"/>
+    <mergeCell ref="J253:J254"/>
+    <mergeCell ref="C223:C224"/>
+    <mergeCell ref="D223:D224"/>
+    <mergeCell ref="E223:E224"/>
+    <mergeCell ref="F223:I223"/>
+    <mergeCell ref="J223:J224"/>
+    <mergeCell ref="C232:C233"/>
+    <mergeCell ref="D232:D233"/>
+    <mergeCell ref="E232:E233"/>
+    <mergeCell ref="F232:I232"/>
+    <mergeCell ref="J232:J233"/>
+    <mergeCell ref="C206:C207"/>
+    <mergeCell ref="D206:D207"/>
+    <mergeCell ref="E206:E207"/>
+    <mergeCell ref="F206:I206"/>
+    <mergeCell ref="J206:J207"/>
+    <mergeCell ref="C215:C216"/>
+    <mergeCell ref="D215:D216"/>
+    <mergeCell ref="E215:E216"/>
+    <mergeCell ref="F215:I215"/>
+    <mergeCell ref="J215:J216"/>
+    <mergeCell ref="C186:C187"/>
+    <mergeCell ref="D186:D187"/>
+    <mergeCell ref="E186:E187"/>
+    <mergeCell ref="F186:I186"/>
+    <mergeCell ref="J186:J187"/>
+    <mergeCell ref="C196:C197"/>
+    <mergeCell ref="D196:D197"/>
+    <mergeCell ref="E196:E197"/>
+    <mergeCell ref="F196:I196"/>
+    <mergeCell ref="J196:J197"/>
+    <mergeCell ref="C149:C150"/>
+    <mergeCell ref="D149:D150"/>
+    <mergeCell ref="E149:E150"/>
+    <mergeCell ref="F149:I149"/>
+    <mergeCell ref="J149:J150"/>
+    <mergeCell ref="C175:C176"/>
+    <mergeCell ref="D175:D176"/>
+    <mergeCell ref="E175:E176"/>
+    <mergeCell ref="F175:I175"/>
+    <mergeCell ref="J175:J176"/>
     <mergeCell ref="C120:C121"/>
     <mergeCell ref="D120:D121"/>
     <mergeCell ref="E120:E121"/>
@@ -9220,71 +9273,89 @@
     <mergeCell ref="J25:J26"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:D15"/>
-    <mergeCell ref="C149:C150"/>
-    <mergeCell ref="D149:D150"/>
-    <mergeCell ref="E149:E150"/>
-    <mergeCell ref="F149:I149"/>
-    <mergeCell ref="J149:J150"/>
-    <mergeCell ref="C175:C176"/>
-    <mergeCell ref="D175:D176"/>
-    <mergeCell ref="E175:E176"/>
-    <mergeCell ref="F175:I175"/>
-    <mergeCell ref="J175:J176"/>
-    <mergeCell ref="C186:C187"/>
-    <mergeCell ref="D186:D187"/>
-    <mergeCell ref="E186:E187"/>
-    <mergeCell ref="F186:I186"/>
-    <mergeCell ref="J186:J187"/>
-    <mergeCell ref="C196:C197"/>
-    <mergeCell ref="D196:D197"/>
-    <mergeCell ref="E196:E197"/>
-    <mergeCell ref="F196:I196"/>
-    <mergeCell ref="J196:J197"/>
-    <mergeCell ref="C206:C207"/>
-    <mergeCell ref="D206:D207"/>
-    <mergeCell ref="E206:E207"/>
-    <mergeCell ref="F206:I206"/>
-    <mergeCell ref="J206:J207"/>
-    <mergeCell ref="C215:C216"/>
-    <mergeCell ref="D215:D216"/>
-    <mergeCell ref="E215:E216"/>
-    <mergeCell ref="F215:I215"/>
-    <mergeCell ref="J215:J216"/>
-    <mergeCell ref="C223:C224"/>
-    <mergeCell ref="D223:D224"/>
-    <mergeCell ref="E223:E224"/>
-    <mergeCell ref="F223:I223"/>
-    <mergeCell ref="J223:J224"/>
-    <mergeCell ref="C232:C233"/>
-    <mergeCell ref="D232:D233"/>
-    <mergeCell ref="E232:E233"/>
-    <mergeCell ref="F232:I232"/>
-    <mergeCell ref="J232:J233"/>
-    <mergeCell ref="C240:C241"/>
-    <mergeCell ref="D240:D241"/>
-    <mergeCell ref="E240:E241"/>
-    <mergeCell ref="F240:I240"/>
-    <mergeCell ref="J240:J241"/>
-    <mergeCell ref="C253:C254"/>
-    <mergeCell ref="D253:D254"/>
-    <mergeCell ref="E253:E254"/>
-    <mergeCell ref="F253:I253"/>
-    <mergeCell ref="J253:J254"/>
-    <mergeCell ref="C282:C283"/>
-    <mergeCell ref="D282:D283"/>
-    <mergeCell ref="E282:E283"/>
-    <mergeCell ref="F282:I282"/>
-    <mergeCell ref="J282:J283"/>
-    <mergeCell ref="C263:C264"/>
-    <mergeCell ref="D263:D264"/>
-    <mergeCell ref="E263:E264"/>
-    <mergeCell ref="F263:I263"/>
-    <mergeCell ref="J263:J264"/>
-    <mergeCell ref="C273:C274"/>
-    <mergeCell ref="D273:D274"/>
-    <mergeCell ref="E273:E274"/>
-    <mergeCell ref="F273:I273"/>
-    <mergeCell ref="J273:J274"/>
+    <mergeCell ref="C139:C140"/>
+    <mergeCell ref="D139:D140"/>
+    <mergeCell ref="E139:E140"/>
+    <mergeCell ref="F139:I139"/>
+    <mergeCell ref="J139:J140"/>
+    <mergeCell ref="C131:C132"/>
+    <mergeCell ref="D131:D132"/>
+    <mergeCell ref="E131:E132"/>
+    <mergeCell ref="F131:I131"/>
+    <mergeCell ref="J131:J132"/>
+    <mergeCell ref="C314:C315"/>
+    <mergeCell ref="D314:D315"/>
+    <mergeCell ref="E314:E315"/>
+    <mergeCell ref="F314:I314"/>
+    <mergeCell ref="J314:J315"/>
+    <mergeCell ref="C306:C307"/>
+    <mergeCell ref="D306:D307"/>
+    <mergeCell ref="E306:E307"/>
+    <mergeCell ref="F306:I306"/>
+    <mergeCell ref="J306:J307"/>
+    <mergeCell ref="C333:C334"/>
+    <mergeCell ref="D333:D334"/>
+    <mergeCell ref="E333:E334"/>
+    <mergeCell ref="F333:I333"/>
+    <mergeCell ref="J333:J334"/>
+    <mergeCell ref="C323:C324"/>
+    <mergeCell ref="D323:D324"/>
+    <mergeCell ref="E323:E324"/>
+    <mergeCell ref="F323:I323"/>
+    <mergeCell ref="J323:J324"/>
+    <mergeCell ref="C363:C364"/>
+    <mergeCell ref="D363:D364"/>
+    <mergeCell ref="E363:E364"/>
+    <mergeCell ref="F363:I363"/>
+    <mergeCell ref="J363:J364"/>
+    <mergeCell ref="C352:C353"/>
+    <mergeCell ref="D352:D353"/>
+    <mergeCell ref="E352:E353"/>
+    <mergeCell ref="F352:I352"/>
+    <mergeCell ref="J352:J353"/>
+    <mergeCell ref="C389:C390"/>
+    <mergeCell ref="D389:D390"/>
+    <mergeCell ref="E389:E390"/>
+    <mergeCell ref="F389:I389"/>
+    <mergeCell ref="J389:J390"/>
+    <mergeCell ref="C377:C378"/>
+    <mergeCell ref="D377:D378"/>
+    <mergeCell ref="E377:E378"/>
+    <mergeCell ref="F377:I377"/>
+    <mergeCell ref="J377:J378"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="J43:J44"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="J32:J33"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="F55:I55"/>
+    <mergeCell ref="J55:J56"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="E66:E67"/>
+    <mergeCell ref="F66:I66"/>
+    <mergeCell ref="J66:J67"/>
+    <mergeCell ref="C99:C100"/>
+    <mergeCell ref="D99:D100"/>
+    <mergeCell ref="E99:E100"/>
+    <mergeCell ref="F99:I99"/>
+    <mergeCell ref="J99:J100"/>
+    <mergeCell ref="D82:D83"/>
+    <mergeCell ref="E82:E83"/>
+    <mergeCell ref="F82:I82"/>
+    <mergeCell ref="J82:J83"/>
+    <mergeCell ref="C82:C83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>